<commit_message>
recursively figure it out 2
</commit_message>
<xml_diff>
--- a/db/PREDICTION.xlsx
+++ b/db/PREDICTION.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Harris\git\fantasyDrafter\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD22916D-1CE6-4871-9C60-83EB62097D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0D089E-D72A-4642-B57B-76E260C19B8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{1CE548C8-74A3-48C1-ACA0-B39B776E85FA}"/>
+    <workbookView xWindow="38280" yWindow="7320" windowWidth="29040" windowHeight="16440" xr2:uid="{1CE548C8-74A3-48C1-ACA0-B39B776E85FA}"/>
   </bookViews>
   <sheets>
     <sheet name="PREDICTION" sheetId="1" r:id="rId1"/>
@@ -3177,19 +3177,19 @@
   </sheetPr>
   <dimension ref="A1:V197"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="Y7" sqref="Y7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="8" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" customWidth="1"/>
+    <col min="2" max="2" width="8" customWidth="1"/>
     <col min="3" max="3" width="6.44140625" style="3" customWidth="1"/>
     <col min="4" max="4" width="8.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.77734375" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="2.44140625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="2.44140625" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.44140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.77734375" bestFit="1" customWidth="1"/>
@@ -3197,8 +3197,8 @@
     <col min="12" max="13" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.33203125" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="12.109375" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="11.33203125" customWidth="1"/>
+    <col min="17" max="17" width="12.109375" customWidth="1"/>
     <col min="18" max="18" width="22.109375" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="16.44140625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="8.6640625" customWidth="1"/>

</xml_diff>